<commit_message>
layout sample analog a/d section, add buttons, battery but not footprints
</commit_message>
<xml_diff>
--- a/kicad/ESP32.xlsx
+++ b/kicad/ESP32.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle2!$A$1:$T$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Tabelle2!$A$1:$T$56</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="269">
   <si>
     <t xml:space="preserve">ESP8266</t>
   </si>
@@ -285,6 +285,9 @@
     <t xml:space="preserve">EMAC_TX_ER</t>
   </si>
   <si>
+    <t xml:space="preserve">GPS EN</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO05</t>
   </si>
   <si>
@@ -549,6 +552,9 @@
     <t xml:space="preserve">HS1_DATA4</t>
   </si>
   <si>
+    <t xml:space="preserve">GPS TXD</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO17</t>
   </si>
   <si>
@@ -564,6 +570,9 @@
     <t xml:space="preserve">HS1_DATA5</t>
   </si>
   <si>
+    <t xml:space="preserve">GPS RXD</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO18</t>
   </si>
   <si>
@@ -681,6 +690,9 @@
     <t xml:space="preserve">EMAC_RXD1</t>
   </si>
   <si>
+    <t xml:space="preserve">KEEPALIVE</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO27</t>
   </si>
   <si>
@@ -699,6 +711,9 @@
     <t xml:space="preserve">EMAC_RX_DV</t>
   </si>
   <si>
+    <t xml:space="preserve">SD_ENABLE*</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO32</t>
   </si>
   <si>
@@ -714,7 +729,10 @@
     <t xml:space="preserve">TOUCH9</t>
   </si>
   <si>
-    <t xml:space="preserve">XTAL_32K_P (32.768kHz crystal oscillator input)</t>
+    <t xml:space="preserve">XTAL_32K_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+3.3VA_ENABLE</t>
   </si>
   <si>
     <t xml:space="preserve">IO33</t>
@@ -732,7 +750,7 @@
     <t xml:space="preserve">TOUCH8</t>
   </si>
   <si>
-    <t xml:space="preserve">XTAL_32K_N (32.768kHz crystal oscillator outut)</t>
+    <t xml:space="preserve">XTAL_32K_N</t>
   </si>
   <si>
     <t xml:space="preserve">IO34</t>
@@ -763,6 +781,9 @@
   </si>
   <si>
     <t xml:space="preserve">ADC1_CH07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTDOWN*</t>
   </si>
   <si>
     <t xml:space="preserve">SENSOR_VP</t>
@@ -1410,13 +1431,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R23" activeCellId="0" sqref="R23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="10.53"/>
@@ -1638,31 +1659,34 @@
       <c r="P6" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="R6" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,16 +1694,16 @@
         <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1687,21 +1711,21 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,16 +1733,16 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1726,21 +1750,21 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,16 +1772,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1765,21 +1789,21 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,16 +1811,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1804,21 +1828,21 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,16 +1850,16 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1843,21 +1867,21 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,16 +1889,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1882,19 +1906,19 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,40 +1926,40 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="R14" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,40 +1967,40 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L15" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="R15" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,40 +2008,40 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="R16" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="S16" s="0"/>
     </row>
@@ -2026,40 +2050,40 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L17" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="R17" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,22 +2091,25 @@
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,22 +2117,25 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,22 +2143,22 @@
         <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="R20" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,25 +2166,25 @@
         <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2162,22 +2192,22 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,25 +2215,25 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,22 +2241,22 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,51 +2264,55 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>211</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="R25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>11</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,25 +2320,28 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,25 +2349,28 @@
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,25 +2378,25 @@
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,22 +2404,22 @@
         <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2387,46 +2427,48 @@
         <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R31" s="5"/>
+        <v>251</v>
+      </c>
+      <c r="R31" s="5" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="R32" s="5"/>
     </row>
@@ -2435,121 +2477,121 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="R33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start switch to 24-bit a/d, smaller buttons, add io expansion, prelim route digital
</commit_message>
<xml_diff>
--- a/kicad/ESP32.xlsx
+++ b/kicad/ESP32.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="270">
   <si>
     <t xml:space="preserve">ESP8266</t>
   </si>
@@ -177,6 +177,9 @@
     <t xml:space="preserve">SD/SDIO/MMC Host Controller</t>
   </si>
   <si>
+    <t xml:space="preserve">Paddle</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO00</t>
   </si>
   <si>
@@ -243,595 +246,595 @@
     <t xml:space="preserve">HSPIWP</t>
   </si>
   <si>
+    <t xml:space="preserve">RXD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U0RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLK_OUT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Console RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS2_DATA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSPIHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_TX_ER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSPICS0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_RX_CLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCK/CLK*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNUSABLE !!! (Flash memory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1CTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPICLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_CLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_CLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDO/SD0*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_DATA0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDI/SD1*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2CTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_DATA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHD/SD2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_DATA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWP/SD3*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1TXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIWP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_DATA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS/CMD*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPICS0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_CMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS2_DATA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSPIQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_TXD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS2_DATA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSPID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_RX_ER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS2_CLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSPICLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_TXD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS2_CMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSPICS0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_RXD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_CLK_OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS TXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2TXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_CLK_OUT_180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSPICLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_DATA7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD SCLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U0CTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSPIQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_TXD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD MISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSPIHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_TX_EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C SDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U0RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSPIWP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_TXD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C SCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSPID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS1_STROBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD MOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_RXD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAC_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_RXD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC2_CH07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAC_RX_DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_CH04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XTAL_32K_P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_CH05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCH8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XTAL_32K_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_CH06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A/D ALERT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_CH07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHUTDOWN*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENSOR_VP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_CH0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC_H</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPS 1PPS</t>
   </si>
   <si>
-    <t xml:space="preserve">RXD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U0RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLK_OUT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Console RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS2_DATA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPIHD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_TX_ER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS EN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSPICS0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_RX_CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCK/CLK*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNUSABLE !!! (Flash memory)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1CTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPICLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDO/SD0*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2RTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPIQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_DATA0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDI/SD1*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2CTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_DATA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHD/SD2*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPIHD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_DATA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SWP/SD3*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1TXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPIWP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_DATA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCS/CMD*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1RTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPICS0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_CMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS2_DATA2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPIQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTDI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_TXD3</t>
+    <t xml:space="preserve">SENSOR_VN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_GPIO03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC1_CH03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“+3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red LED</t>
   </si>
   <si>
     <t xml:space="preserve">Yellow LED</t>
   </si>
   <si>
-    <t xml:space="preserve">IO13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS2_DATA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_RX_ER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS2_CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPICLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_TXD2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Green LED</t>
   </si>
   <si>
-    <t xml:space="preserve">IO15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS2_CMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSPICS0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_RXD3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blue LED</t>
   </si>
   <si>
-    <t xml:space="preserve">IO16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_CLK_OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS TXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2TXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_CLK_OUT_180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS RXD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSPICLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_DATA7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD SCLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U0CTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSPIQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_TXD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD MISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSPIHD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_TX_EN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C SDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U0RTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSPIWP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_TXD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C SCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSPID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HS1_STROBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD MOSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAC_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_RXD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAC_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_RXD1</t>
+    <t xml:space="preserve">+3.3VA_ENABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS ENABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_ENABLE*</t>
   </si>
   <si>
     <t xml:space="preserve">KEEPALIVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC2_CH07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMAC_RX_DV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_ENABLE*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC1_CH04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XTAL_32K_P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+3.3VA_ENABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC1_CH05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOUCH8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XTAL_32K_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC1_CH06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A/D ALERT0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IO35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC1_CH07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHUTDOWN*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SENSOR_VP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC1_CH0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC_H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SENSOR_VN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTC_GPIO03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC1_CH03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3V3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“+3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NC</t>
   </si>
 </sst>
 </file>
@@ -1431,10 +1434,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1444,11 +1447,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="2" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="2" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="2" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="13" style="2" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="2" width="9.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="14.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="17.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="11.99"/>
@@ -1508,37 +1512,40 @@
       <c r="P1" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,25 +1553,25 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,35 +1579,33 @@
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>72</v>
-      </c>
+      <c r="R4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -1610,7 +1615,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>74</v>
@@ -1633,7 +1638,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>79</v>
@@ -1658,9 +1663,6 @@
       </c>
       <c r="P6" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,25 +1670,25 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,16 +1696,16 @@
         <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1711,21 +1713,22 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,16 +1736,16 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1750,21 +1753,22 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,16 +1776,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1789,21 +1793,22 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>100</v>
+        <v>111</v>
+      </c>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,16 +1816,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1828,21 +1833,22 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>100</v>
+        <v>117</v>
+      </c>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,16 +1856,16 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1867,21 +1873,22 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>100</v>
+        <v>123</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,16 +1896,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1906,19 +1913,20 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>100</v>
+        <v>128</v>
+      </c>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,123 +1934,117 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="P14" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>139</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="R14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="P15" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>149</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="R15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="P16" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>159</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="R16" s="0"/>
       <c r="S16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,40 +2052,37 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="P17" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,25 +2090,25 @@
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,25 +2116,25 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,22 +2142,22 @@
         <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="R20" s="0" t="s">
-        <v>186</v>
+        <v>180</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,25 +2165,25 @@
         <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,22 +2191,22 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,25 +2214,25 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,22 +2240,22 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,139 +2263,132 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="O25" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="R25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>11</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>221</v>
-      </c>
+      <c r="R26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>228</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="R27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>235</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="R28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,22 +2396,22 @@
         <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,22 +2419,22 @@
         <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="R31" s="5" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,52 +2442,54 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="R32" s="5"/>
+        <v>249</v>
+      </c>
+      <c r="R32" s="5" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="R33" s="5"/>
     </row>
@@ -2504,13 +2498,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,13 +2512,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,13 +2526,13 @@
         <v>3</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,13 +2540,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,10 +2554,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,13 +2565,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,13 +2579,54 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q43" s="0"/>
+      <c r="R43" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R44" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="R40" s="2" t="s">
-        <v>262</v>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R45" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R46" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R47" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R48" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R49" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R50" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix up digital connections - not done
</commit_message>
<xml_diff>
--- a/kicad/ESP32.xlsx
+++ b/kicad/ESP32.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="285">
   <si>
     <t xml:space="preserve">ESP8266</t>
   </si>
@@ -222,7 +222,7 @@
     <t xml:space="preserve">CLK_OUT3</t>
   </si>
   <si>
-    <t xml:space="preserve">Console TXD</t>
+    <t xml:space="preserve">TXD_CON</t>
   </si>
   <si>
     <t xml:space="preserve">IO02</t>
@@ -246,6 +246,9 @@
     <t xml:space="preserve">HSPIWP</t>
   </si>
   <si>
+    <t xml:space="preserve">AN3_CS*</t>
+  </si>
+  <si>
     <t xml:space="preserve">RXD0</t>
   </si>
   <si>
@@ -258,7 +261,7 @@
     <t xml:space="preserve">CLK_OUT2</t>
   </si>
   <si>
-    <t xml:space="preserve">Console RXD</t>
+    <t xml:space="preserve">RXD_CON</t>
   </si>
   <si>
     <t xml:space="preserve">IO04</t>
@@ -285,6 +288,9 @@
     <t xml:space="preserve">EMAC_TX_ER</t>
   </si>
   <si>
+    <t xml:space="preserve">KEEPALIVE</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO05</t>
   </si>
   <si>
@@ -675,6 +681,9 @@
     <t xml:space="preserve">EMAC_RXD1</t>
   </si>
   <si>
+    <t xml:space="preserve">BLINK</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO27</t>
   </si>
   <si>
@@ -693,6 +702,9 @@
     <t xml:space="preserve">EMAC_RX_DV</t>
   </si>
   <si>
+    <t xml:space="preserve">CS0*</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO32</t>
   </si>
   <si>
@@ -711,6 +723,9 @@
     <t xml:space="preserve">XTAL_32K_P</t>
   </si>
   <si>
+    <t xml:space="preserve">CS1*</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO33</t>
   </si>
   <si>
@@ -729,6 +744,9 @@
     <t xml:space="preserve">XTAL_32K_N</t>
   </si>
   <si>
+    <t xml:space="preserve">CS2*</t>
+  </si>
+  <si>
     <t xml:space="preserve">IO34</t>
   </si>
   <si>
@@ -813,28 +831,55 @@
     <t xml:space="preserve">NC</t>
   </si>
   <si>
+    <t xml:space="preserve">TCA9534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Red LED</t>
   </si>
   <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yellow LED</t>
   </si>
   <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Green LED</t>
   </si>
   <si>
+    <t xml:space="preserve">P3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blue LED</t>
   </si>
   <si>
+    <t xml:space="preserve">P4</t>
+  </si>
+  <si>
     <t xml:space="preserve">+3.3VA_ENABLE</t>
   </si>
   <si>
+    <t xml:space="preserve">P5</t>
+  </si>
+  <si>
     <t xml:space="preserve">GPS ENABLE</t>
   </si>
   <si>
+    <t xml:space="preserve">P6</t>
+  </si>
+  <si>
     <t xml:space="preserve">SD_ENABLE*</t>
   </si>
   <si>
-    <t xml:space="preserve">KEEPALIVE</t>
+    <t xml:space="preserve">P7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AN_REFSEL</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1482,7 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1605,29 +1650,31 @@
       <c r="P4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="R4" s="0"/>
+      <c r="R4" s="0" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,60 +1682,64 @@
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="R6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,16 +1747,16 @@
         <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1713,22 +1764,22 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,16 +1787,16 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1753,22 +1804,22 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,16 +1827,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1793,22 +1844,22 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,16 +1867,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1833,22 +1884,22 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,16 +1907,16 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1873,22 +1924,22 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,16 +1947,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1913,20 +1964,20 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,37 +1985,37 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="R14" s="0"/>
     </row>
@@ -1973,37 +2024,37 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="R15" s="0"/>
     </row>
@@ -2012,37 +2063,37 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="M16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="R16" s="0"/>
       <c r="S16" s="0"/>
@@ -2052,37 +2103,37 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="M17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,25 +2141,25 @@
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,25 +2167,25 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,22 +2193,22 @@
         <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,25 +2216,25 @@
         <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,22 +2242,22 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,25 +2265,25 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,22 +2291,22 @@
         <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,233 +2314,284 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="R25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>11</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="R26" s="0"/>
+        <v>217</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="R27" s="0"/>
+        <v>224</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="S27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="R28" s="0"/>
+        <v>231</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>233</v>
+        <v>238</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>238</v>
-      </c>
+      <c r="B30" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
       <c r="R30" s="5" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+      <c r="A31" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B31" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>243</v>
-      </c>
+      <c r="D31" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
       <c r="R31" s="5" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+      <c r="A32" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>249</v>
+      <c r="B32" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="n">
+      <c r="A33" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>249</v>
+      <c r="B33" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="R33" s="5"/>
     </row>
@@ -2498,13 +2600,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,13 +2614,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,13 +2628,13 @@
         <v>3</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,13 +2642,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,10 +2656,10 @@
         <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,13 +2667,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,54 +2681,80 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q43" s="0"/>
+      <c r="L43" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>269</v>
+      </c>
       <c r="R43" s="2" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q44" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="R44" s="2" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q45" s="0" t="s">
+        <v>273</v>
+      </c>
       <c r="R45" s="2" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q46" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="R46" s="2" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q47" s="0" t="s">
+        <v>277</v>
+      </c>
       <c r="R47" s="2" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q48" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="R48" s="0" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q49" s="0" t="s">
+        <v>281</v>
+      </c>
       <c r="R49" s="2" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q50" s="2" t="s">
+        <v>283</v>
+      </c>
       <c r="R50" s="2" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix up names, digital signals, finish reference
</commit_message>
<xml_diff>
--- a/kicad/ESP32.xlsx
+++ b/kicad/ESP32.xlsx
@@ -543,7 +543,7 @@
     <t xml:space="preserve">HS1_DATA4</t>
   </si>
   <si>
-    <t xml:space="preserve">GPS TXD</t>
+    <t xml:space="preserve">RXD_GPS</t>
   </si>
   <si>
     <t xml:space="preserve">IO17</t>
@@ -561,7 +561,7 @@
     <t xml:space="preserve">HS1_DATA5</t>
   </si>
   <si>
-    <t xml:space="preserve">GPS RXD</t>
+    <t xml:space="preserve">TXD_GPS</t>
   </si>
   <si>
     <t xml:space="preserve">IO18</t>
@@ -1482,7 +1482,7 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+      <selection pane="topLeft" activeCell="R19" activeCellId="0" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2161,6 +2161,7 @@
       <c r="R18" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="S18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -2187,6 +2188,7 @@
       <c r="R19" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="S19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">

</xml_diff>